<commit_message>
Need to add game logic for human going first. Need to add autoplay function.
</commit_message>
<xml_diff>
--- a/DecisionTree.xlsx
+++ b/DecisionTree.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="19980" windowHeight="7065"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="19980" windowHeight="7065" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ComputerFirst" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
   <si>
     <t>MV1: Cell (x = 8)</t>
   </si>
@@ -107,22 +107,28 @@
     <t>HUMAN FIRST</t>
   </si>
   <si>
-    <t>MV2: Cell (x = 5)</t>
+    <t>Alternative 1</t>
   </si>
   <si>
-    <t>MV1</t>
+    <t>Alternative 2</t>
   </si>
   <si>
-    <t>MV2</t>
+    <t>MV2: Cell (y = 0 % 2)</t>
   </si>
   <si>
-    <t>MV3</t>
+    <t>winOrBlock()</t>
   </si>
   <si>
-    <t>MV4</t>
+    <t>MV3: Cell (y = 0 % 2)</t>
   </si>
   <si>
-    <t>MV5</t>
+    <t>MV3: Cell (y = 1 % 2)</t>
+  </si>
+  <si>
+    <t>HUMAN</t>
+  </si>
+  <si>
+    <t>COMP</t>
   </si>
 </sst>
 </file>
@@ -162,7 +168,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,6 +193,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -200,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -210,7 +222,17 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2982,13 +3004,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3041,13 +3063,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3085,13 +3107,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3127,159 +3149,27 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Branch 3"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1238250" y="3429000"/>
-          <a:ext cx="1285875" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>23813</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>138113</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="95" name="Leaf 1"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4486275" y="633413"/>
-          <a:ext cx="0" cy="114300"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>23813</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>138113</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="97" name="Leaf 2"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4486275" y="1243013"/>
-          <a:ext cx="0" cy="114300"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="100" name="TrNd 3"/>
+        <xdr:cNvPr id="6" name="TrNd 1"/>
         <xdr:cNvSpPr>
           <a:spLocks/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2733675" y="1828800"/>
+          <a:off x="2733675" y="609600"/>
           <a:ext cx="161925" cy="161925"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3320,23 +3210,170 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Branch 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3143250" y="685800"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TrNd 11"/>
+        <xdr:cNvSpPr>
+          <a:spLocks/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4486275" y="609600"/>
+          <a:ext cx="161925" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="9999FF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Branch 111"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4895850" y="685800"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="105" name="Branch 31"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3143250" y="1905000"/>
+        <xdr:cNvPr id="19" name="Branch 112"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4895850" y="1295400"/>
           <a:ext cx="1343025" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -3362,25 +3399,451 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="TrNd 111"/>
+        <xdr:cNvSpPr>
+          <a:spLocks/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6238875" y="609600"/>
+          <a:ext cx="161925" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="9999FF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="69" name="FBranch 1111"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6400800" y="685800"/>
+          <a:ext cx="247650" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="70" name="Branch 1111"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6648450" y="685800"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="71" name="Leaf 1111"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7991475" y="628650"/>
+          <a:ext cx="0" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="72" name="FBranch 1112"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6400800" y="990600"/>
+          <a:ext cx="247650" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="73" name="Branch 1112"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6648450" y="1295400"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="74" name="Leaf 1112"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7991475" y="1238250"/>
+          <a:ext cx="0" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="76" name="TrNd 112"/>
+        <xdr:cNvSpPr>
+          <a:spLocks/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6238875" y="1828800"/>
+          <a:ext cx="161925" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="9999FF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="87" name="Branch 1121"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6648450" y="2514600"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="106" name="Leaf 31"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4486275" y="1847850"/>
+        <xdr:cNvPr id="88" name="Leaf 1121"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7991475" y="2457450"/>
           <a:ext cx="0" cy="114300"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -3406,113 +3869,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="110" name="XBranch 1"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2733675" y="685800"/>
-          <a:ext cx="1752600" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="111" name="XBranch 2"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2733675" y="1295400"/>
-          <a:ext cx="1752600" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>80963</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="112" name="FBranch 31"/>
+        <xdr:cNvPr id="89" name="FBranch 1121"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="2895600" y="1905000"/>
+          <a:off x="6400800" y="1905000"/>
           <a:ext cx="247650" cy="4763"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -3538,26 +3913,1069 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="90" name="FBranch 111"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4648200" y="990600"/>
+          <a:ext cx="247650" cy="461963"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="91" name="FBranch 112"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4648200" y="1452563"/>
+          <a:ext cx="247650" cy="452437"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="92" name="FBranch 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2895600" y="1447800"/>
+          <a:ext cx="247650" cy="4763"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="155" name="Branch 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1238250" y="3124200"/>
+          <a:ext cx="1495425" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="161" name="TrNd 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2733675" y="2438400"/>
+          <a:ext cx="161925" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="9999FF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="169" name="Branch 21"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3143250" y="3124200"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="177" name="TrNd 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2733675" y="3048000"/>
+          <a:ext cx="161925" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="9999FF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="182" name="Branch 31"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3143250" y="3733800"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="190" name="TrNd 21"/>
+        <xdr:cNvSpPr>
+          <a:spLocks/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4486275" y="2438400"/>
+          <a:ext cx="161925" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="9999FF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="196" name="Branch 211"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4895850" y="2514600"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="199" name="Branch 212"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4895850" y="3124200"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="203" name="TrNd 211"/>
+        <xdr:cNvSpPr>
+          <a:spLocks/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6238875" y="2438400"/>
+          <a:ext cx="161925" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="9999FF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="214" name="Branch 2111"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6648450" y="3124200"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="215" name="Leaf 2111"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7991475" y="3067050"/>
+          <a:ext cx="0" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="216" name="FBranch 2111"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6400800" y="2514600"/>
+          <a:ext cx="247650" cy="4763"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="223" name="TrNd 212"/>
+        <xdr:cNvSpPr>
+          <a:spLocks/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6238875" y="3048000"/>
+          <a:ext cx="161925" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="9999FF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="234" name="Branch 2121"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6648450" y="3733800"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="235" name="Leaf 2121"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7991475" y="3676650"/>
+          <a:ext cx="0" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="236" name="FBranch 2121"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6400800" y="3124200"/>
+          <a:ext cx="247650" cy="4763"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="237" name="FBranch 211"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4648200" y="2514600"/>
+          <a:ext cx="247650" cy="309563"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="238" name="FBranch 212"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4648200" y="2824163"/>
+          <a:ext cx="247650" cy="300037"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="239" name="FBranch 21"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2895600" y="2819400"/>
+          <a:ext cx="247650" cy="4763"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>80963</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="113" name="FBranch 1"/>
+        <xdr:cNvPr id="240" name="FBranch 1"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="990600" y="685800"/>
-          <a:ext cx="247650" cy="614363"/>
+          <a:off x="990600" y="1447800"/>
+          <a:ext cx="247650" cy="1223963"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3584,23 +5002,170 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="241" name="FBranch 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="990600" y="2671763"/>
+          <a:ext cx="247650" cy="147637"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>80963</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="114" name="FBranch 2"/>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="242" name="FBranch 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="990600" y="2671763"/>
+          <a:ext cx="247650" cy="1062037"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="243" name="TrNd 31"/>
+        <xdr:cNvSpPr>
+          <a:spLocks/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4486275" y="3657600"/>
+          <a:ext cx="161925" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="9999FF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="244" name="FBranch 31"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="990600" y="1295400"/>
+          <a:off x="2895600" y="4038600"/>
           <a:ext cx="247650" cy="4763"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -3626,26 +5191,334 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>80963</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="115" name="FBranch 3"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="990600" y="1300163"/>
-          <a:ext cx="247650" cy="604837"/>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="245" name="FBranch 311"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4648200" y="3733800"/>
+          <a:ext cx="247650" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="246" name="Branch 311"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4895850" y="3733800"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="247" name="Leaf 311"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8534400" y="3676650"/>
+          <a:ext cx="0" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="248" name="FBranch 312"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4648200" y="4038600"/>
+          <a:ext cx="247650" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="249" name="Branch 312"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4895850" y="4343400"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="250" name="Leaf 312"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8534400" y="4286250"/>
+          <a:ext cx="0" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="251" name="XBranch 311"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6238875" y="3733800"/>
+          <a:ext cx="2295525" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="252" name="XBranch 312"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6238875" y="4343400"/>
+          <a:ext cx="2295525" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3960,7 +5833,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3968,17 +5843,17 @@
     <col min="2" max="2" width="2.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="3.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="3.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="4.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="2.42578125" style="1" customWidth="1"/>
     <col min="13" max="13" width="3.7109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="4.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="2.42578125" style="1" customWidth="1"/>
     <col min="18" max="18" width="3.7109375" style="1" customWidth="1"/>
@@ -3996,19 +5871,19 @@
   <sheetData>
     <row r="1" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>32</v>
+        <v>37</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="V1" s="2" t="s">
         <v>3</v>
@@ -4026,7 +5901,7 @@
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="E3" s="14"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -4036,7 +5911,7 @@
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
+      <c r="O3" s="14"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
@@ -4050,7 +5925,7 @@
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="E4" s="14"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -4063,7 +5938,7 @@
         <f>IF($K$8=$W$5,"&gt;&gt;&gt;","")</f>
         <v>&gt;&gt;&gt;</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="14" t="s">
         <v>8</v>
       </c>
       <c r="P4" s="4"/>
@@ -4078,7 +5953,7 @@
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="E5" s="14"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -4088,7 +5963,7 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
+      <c r="O5" s="14"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
@@ -4113,7 +5988,7 @@
         <f>IF($A$20=$F$8,"&gt;&gt;&gt;","")</f>
         <v>&gt;&gt;&gt;</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="14" t="s">
         <v>1</v>
       </c>
       <c r="H6" s="4"/>
@@ -4128,7 +6003,7 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
+      <c r="O6" s="14"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
@@ -4148,7 +6023,7 @@
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
+      <c r="O7" s="14"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
@@ -4162,7 +6037,7 @@
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
-      <c r="E8" s="3">
+      <c r="E8" s="15">
         <f>$F$8</f>
         <v>0</v>
       </c>
@@ -4182,7 +6057,7 @@
         <f>IF($K$8=$W$9,"&gt;&gt;&gt;","")</f>
         <v>&gt;&gt;&gt;</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="O8" s="14" t="s">
         <v>9</v>
       </c>
       <c r="AA8" s="3"/>
@@ -4190,7 +6065,7 @@
     <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
-      <c r="E9" s="3"/>
+      <c r="E9" s="15"/>
       <c r="V9" s="5">
         <v>0</v>
       </c>
@@ -4206,7 +6081,7 @@
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
-      <c r="E10" s="3"/>
+      <c r="E10" s="15"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
@@ -4220,7 +6095,7 @@
         <f>IF($K$16=$W$13,"&gt;&gt;&gt;","")</f>
         <v>&gt;&gt;&gt;</v>
       </c>
-      <c r="O12" s="4" t="s">
+      <c r="O12" s="14" t="s">
         <v>12</v>
       </c>
       <c r="V12" s="3"/>
@@ -4246,7 +6121,7 @@
         <f>IF($A$20=$F$16,"&gt;&gt;&gt;","")</f>
         <v>&gt;&gt;&gt;</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="14" t="s">
         <v>2</v>
       </c>
       <c r="I14" s="4" t="str">
@@ -4267,7 +6142,7 @@
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
-      <c r="E16" s="3">
+      <c r="E16" s="15">
         <f>$F$16</f>
         <v>0</v>
       </c>
@@ -4287,7 +6162,7 @@
         <f>IF($K$16=$P$18,"&gt;&gt;&gt;","")</f>
         <v>&gt;&gt;&gt;</v>
       </c>
-      <c r="O16" s="4" t="s">
+      <c r="O16" s="14" t="s">
         <v>13</v>
       </c>
       <c r="S16" s="4" t="str">
@@ -4303,7 +6178,7 @@
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
-      <c r="E17" s="3"/>
+      <c r="E17" s="15"/>
       <c r="V17" s="7">
         <v>0</v>
       </c>
@@ -4316,8 +6191,8 @@
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="E18" s="3"/>
-      <c r="O18" s="3">
+      <c r="E18" s="15"/>
+      <c r="O18" s="15">
         <f>$P$18</f>
         <v>0</v>
       </c>
@@ -4342,7 +6217,7 @@
         <f>IF($K$24=$W$21,"&gt;&gt;&gt;","")</f>
         <v>&gt;&gt;&gt;</v>
       </c>
-      <c r="O20" s="4" t="s">
+      <c r="O20" s="14" t="s">
         <v>17</v>
       </c>
       <c r="V20" s="3"/>
@@ -4369,7 +6244,7 @@
         <f>IF($A$20=$F$24,"&gt;&gt;&gt;","")</f>
         <v>&gt;&gt;&gt;</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="14" t="s">
         <v>15</v>
       </c>
       <c r="I22" s="4" t="str">
@@ -4387,7 +6262,7 @@
       <c r="W23" s="3"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="E24" s="3">
+      <c r="E24" s="15">
         <f>$F$24</f>
         <v>0</v>
       </c>
@@ -4407,12 +6282,12 @@
         <f>IF($K$24=$W$25,"&gt;&gt;&gt;","")</f>
         <v>&gt;&gt;&gt;</v>
       </c>
-      <c r="O24" s="4" t="s">
+      <c r="O24" s="14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="E25" s="3"/>
+      <c r="E25" s="15"/>
       <c r="V25" s="7">
         <v>0</v>
       </c>
@@ -4425,7 +6300,7 @@
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="E26" s="3"/>
+      <c r="E26" s="15"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="V27" s="3"/>
@@ -4436,7 +6311,7 @@
         <f>IF($K$32=$W$29,"&gt;&gt;&gt;","")</f>
         <v>&gt;&gt;&gt;</v>
       </c>
-      <c r="O28" s="4" t="s">
+      <c r="O28" s="14" t="s">
         <v>19</v>
       </c>
       <c r="V28" s="3"/>
@@ -4459,7 +6334,7 @@
         <f>IF($A$20=$F$32,"&gt;&gt;&gt;","")</f>
         <v>&gt;&gt;&gt;</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="14" t="s">
         <v>16</v>
       </c>
       <c r="I30" s="4" t="str">
@@ -4477,7 +6352,7 @@
       <c r="W31" s="3"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="E32" s="3">
+      <c r="E32" s="15">
         <f>$F$32</f>
         <v>0</v>
       </c>
@@ -4497,12 +6372,12 @@
         <f>IF($K$32=$W$33,"&gt;&gt;&gt;","")</f>
         <v>&gt;&gt;&gt;</v>
       </c>
-      <c r="O32" s="4" t="s">
+      <c r="O32" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="33" spans="5:24" x14ac:dyDescent="0.2">
-      <c r="E33" s="3"/>
+      <c r="E33" s="15"/>
       <c r="V33" s="7">
         <v>0</v>
       </c>
@@ -4515,7 +6390,7 @@
       </c>
     </row>
     <row r="34" spans="5:24" x14ac:dyDescent="0.2">
-      <c r="E34" s="3"/>
+      <c r="E34" s="15"/>
     </row>
     <row r="35" spans="5:24" x14ac:dyDescent="0.2">
       <c r="V35" s="3"/>
@@ -4530,73 +6405,91 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF27"/>
+  <dimension ref="A1:AP91"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="V25" sqref="V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="3.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="3.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="4.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" style="1" customWidth="1"/>
-    <col min="12" max="13" width="4.85546875" style="1" customWidth="1"/>
+    <col min="10" max="11" width="7.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="2.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="3.7109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="4.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="2.42578125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="3.7109375" style="1" customWidth="1"/>
     <col min="19" max="19" width="4.7109375" style="1" customWidth="1"/>
     <col min="20" max="20" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.7109375" style="1" customWidth="1"/>
-    <col min="23" max="23" width="10.7109375" style="1" customWidth="1"/>
-    <col min="24" max="24" width="4.7109375" style="1" customWidth="1"/>
-    <col min="25" max="26" width="7.7109375" style="1" customWidth="1"/>
-    <col min="27" max="28" width="4.140625" style="1" customWidth="1"/>
-    <col min="29" max="29" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.7109375" style="1" customWidth="1"/>
-    <col min="32" max="32" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.7109375" style="1" customWidth="1"/>
+    <col min="22" max="23" width="4.85546875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.7109375" style="1" customWidth="1"/>
+    <col min="28" max="28" width="10.7109375" style="1" customWidth="1"/>
+    <col min="29" max="29" width="4.7109375" style="1" customWidth="1"/>
+    <col min="30" max="30" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.7109375" style="1" customWidth="1"/>
     <col min="33" max="33" width="10.7109375" style="1" customWidth="1"/>
-    <col min="34" max="16384" width="9.140625" style="1"/>
+    <col min="34" max="34" width="4.7109375" style="1" customWidth="1"/>
+    <col min="35" max="36" width="7.7109375" style="1" customWidth="1"/>
+    <col min="37" max="38" width="4.140625" style="1" customWidth="1"/>
+    <col min="39" max="39" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="7.7109375" style="1" customWidth="1"/>
+    <col min="42" max="42" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.7109375" style="1" customWidth="1"/>
+    <col min="44" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="L1" s="2" t="s">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="E1" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
       <c r="AA1" s="2"/>
       <c r="AB1" s="2"/>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="AC2" s="4"/>
-      <c r="AD2" s="4"/>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="AM2" s="4"/>
+      <c r="AN2" s="4"/>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -4606,7 +6499,6 @@
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
@@ -4618,26 +6510,44 @@
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
       <c r="Z3" s="4"/>
-      <c r="AF3" s="3"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="4"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="4"/>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="4"/>
+      <c r="AP3" s="3"/>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A4" s="10"/>
       <c r="B4" s="4"/>
-      <c r="D4" s="4" t="str">
-        <f>IF($A$10=$M$5,"&gt;&gt;&gt;","")</f>
-        <v>&gt;&gt;&gt;</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
+      <c r="O4" s="14"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
+      <c r="S4" s="4" t="str">
+        <f>IF($P$8=$W$5,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="U4" s="4"/>
       <c r="V4" s="4"/>
       <c r="W4" s="4"/>
@@ -4647,34 +6557,84 @@
       <c r="AA4" s="4"/>
       <c r="AB4" s="4"/>
       <c r="AC4" s="4"/>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="4"/>
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="4"/>
+      <c r="AH4" s="4"/>
+      <c r="AI4" s="4"/>
+      <c r="AJ4" s="4"/>
+      <c r="AK4" s="4"/>
+      <c r="AL4" s="4"/>
+      <c r="AM4" s="4"/>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A5" s="10"/>
       <c r="B5" s="4"/>
-      <c r="L5" s="9">
-        <v>0</v>
-      </c>
-      <c r="M5" s="9">
-        <f>$L$5</f>
-        <v>0</v>
-      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
       <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
+      <c r="O5" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4"/>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
+      <c r="V5" s="5">
+        <v>0</v>
+      </c>
+      <c r="W5" s="5">
+        <f>$V$9</f>
+        <v>0</v>
+      </c>
+      <c r="X5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="4"/>
+      <c r="AC5" s="4"/>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="4"/>
+      <c r="AG5" s="4"/>
+      <c r="AH5" s="4"/>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A6" s="10"/>
       <c r="B6" s="4"/>
-      <c r="E6" s="3"/>
-      <c r="O6" s="3"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4" t="str">
+        <f>IF($K$11=$P$8,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
@@ -4688,18 +6648,42 @@
       <c r="AB6" s="4"/>
       <c r="AC6" s="4"/>
       <c r="AD6" s="4"/>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
+      <c r="AE6" s="4"/>
+      <c r="AF6" s="4"/>
+      <c r="AG6" s="4"/>
+      <c r="AH6" s="4"/>
+      <c r="AI6" s="4"/>
+      <c r="AJ6" s="4"/>
+      <c r="AK6" s="4"/>
+      <c r="AL6" s="4"/>
+      <c r="AM6" s="4"/>
+      <c r="AN6" s="4"/>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
       <c r="B7" s="4"/>
-      <c r="E7" s="4" t="s">
-        <v>27</v>
-      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
+      <c r="T7" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
+      <c r="V7" s="3"/>
       <c r="W7" s="4"/>
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
@@ -4707,334 +6691,844 @@
       <c r="AA7" s="4"/>
       <c r="AB7" s="4"/>
       <c r="AC7" s="4"/>
-      <c r="AF7" s="3"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="D8" s="4" t="str">
-        <f>IF($A$10=$M$9,"&gt;&gt;&gt;","")</f>
+      <c r="AD7" s="4"/>
+      <c r="AE7" s="4"/>
+      <c r="AF7" s="4"/>
+      <c r="AG7" s="4"/>
+      <c r="AH7" s="4"/>
+      <c r="AI7" s="4"/>
+      <c r="AJ7" s="4"/>
+      <c r="AK7" s="4"/>
+      <c r="AL7" s="4"/>
+      <c r="AM7" s="4"/>
+      <c r="AP7" s="3"/>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A8" s="10"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="4">
+        <f>MAX($W$5,$W$9)</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4" t="str">
+        <f>IF($P$8=$W$9,"&gt;&gt;&gt;","")</f>
         <v>&gt;&gt;&gt;</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
+      <c r="T8" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="4"/>
-      <c r="Z8" s="4"/>
-      <c r="AA8" s="4"/>
+      <c r="Y8" s="3"/>
       <c r="AB8" s="4"/>
       <c r="AC8" s="4"/>
-      <c r="AF8" s="3"/>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="L9" s="9">
-        <v>0</v>
-      </c>
-      <c r="M9" s="9">
-        <f>$L$9</f>
-        <v>0</v>
-      </c>
+      <c r="AD8" s="4"/>
+      <c r="AE8" s="4"/>
+      <c r="AF8" s="4"/>
+      <c r="AG8" s="4"/>
+      <c r="AH8" s="4"/>
+      <c r="AI8" s="4"/>
+      <c r="AJ8" s="4"/>
+      <c r="AK8" s="4"/>
+      <c r="AL8" s="4"/>
+      <c r="AM8" s="4"/>
+      <c r="AP8" s="3"/>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A9" s="10"/>
+      <c r="B9" s="4"/>
+      <c r="D9" s="4" t="str">
+        <f>IF($A$19=$F$11,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4" t="str">
+        <f>IF($F$11=$K$11,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
       <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
+      <c r="O9" s="14"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
-      <c r="V9" s="4"/>
-      <c r="W9" s="4"/>
-      <c r="X9" s="4"/>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <f>MAX($M$5,$M$9,$F$14)</f>
+      <c r="V9" s="5">
         <v>0</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="O10" s="3"/>
+      <c r="W9" s="5">
+        <f>$V$9</f>
+        <v>0</v>
+      </c>
+      <c r="X9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y9" s="3"/>
+      <c r="AB9" s="4"/>
+      <c r="AC9" s="4"/>
+      <c r="AD9" s="4"/>
+      <c r="AE9" s="4"/>
+      <c r="AF9" s="4"/>
+      <c r="AG9" s="4"/>
+      <c r="AH9" s="4"/>
+    </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A10" s="10"/>
+      <c r="B10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
-      <c r="X10" s="4"/>
-      <c r="Y10" s="4"/>
-      <c r="Z10" s="4"/>
-      <c r="AA10" s="4"/>
+      <c r="Y10" s="3"/>
       <c r="AB10" s="4"/>
       <c r="AC10" s="4"/>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
-        <f>$A$10</f>
+      <c r="AD10" s="4"/>
+      <c r="AE10" s="4"/>
+      <c r="AF10" s="4"/>
+      <c r="AG10" s="4"/>
+      <c r="AH10" s="4"/>
+      <c r="AI10" s="4"/>
+      <c r="AJ10" s="4"/>
+      <c r="AK10" s="4"/>
+      <c r="AL10" s="4"/>
+      <c r="AM10" s="4"/>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A11" s="10"/>
+      <c r="B11" s="4"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="1">
+        <f>MAX($K$11)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="K11" s="1">
+        <f>MAX($P$8,$P$14)</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="14" t="s">
         <v>28</v>
       </c>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
-      <c r="V11" s="4"/>
+      <c r="V11" s="3"/>
       <c r="W11" s="4"/>
-      <c r="X11" s="4"/>
-      <c r="Y11" s="4"/>
-      <c r="Z11" s="4"/>
-      <c r="AA11" s="4"/>
       <c r="AB11" s="4"/>
       <c r="AC11" s="4"/>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="D12" s="4" t="str">
-        <f>IF($A$10=$F$14,"&gt;&gt;&gt;","")</f>
+      <c r="AD11" s="4"/>
+      <c r="AE11" s="4"/>
+      <c r="AF11" s="4"/>
+      <c r="AG11" s="4"/>
+      <c r="AH11" s="4"/>
+      <c r="AI11" s="4"/>
+      <c r="AJ11" s="4"/>
+      <c r="AK11" s="4"/>
+      <c r="AL11" s="4"/>
+      <c r="AM11" s="4"/>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A12" s="10"/>
+      <c r="B12" s="4"/>
+      <c r="E12" s="15"/>
+      <c r="N12" s="4" t="str">
+        <f>IF($K$11=$P$14,"&gt;&gt;&gt;","")</f>
         <v>&gt;&gt;&gt;</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12" s="4" t="str">
-        <f>IF($F$14=$M$13,"&gt;&gt;&gt;","")</f>
+      <c r="O12" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="S12" s="4" t="str">
+        <f>IF($P$14=$W$13,"&gt;&gt;&gt;","")</f>
         <v>&gt;&gt;&gt;</v>
       </c>
-      <c r="J12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="4"/>
-      <c r="V12" s="4"/>
+      <c r="T12" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="W12" s="4"/>
-      <c r="X12" s="4"/>
-      <c r="Y12" s="4"/>
-      <c r="Z12" s="4"/>
-      <c r="AA12" s="4"/>
       <c r="AB12" s="4"/>
       <c r="AC12" s="4"/>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="L13" s="3">
+      <c r="AD12" s="4"/>
+      <c r="AE12" s="4"/>
+      <c r="AF12" s="4"/>
+      <c r="AG12" s="4"/>
+      <c r="AH12" s="4"/>
+      <c r="AI12" s="4"/>
+      <c r="AJ12" s="4"/>
+      <c r="AK12" s="4"/>
+      <c r="AL12" s="4"/>
+      <c r="AM12" s="4"/>
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A13" s="10"/>
+      <c r="B13" s="4"/>
+      <c r="E13" s="15"/>
+      <c r="V13" s="5">
         <v>0</v>
       </c>
-      <c r="M13" s="3">
-        <f>$L$13</f>
+      <c r="W13" s="5">
+        <f>$V$9</f>
         <v>0</v>
       </c>
-      <c r="R13" s="3"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
-      <c r="V13" s="4"/>
-      <c r="W13" s="4"/>
-      <c r="X13" s="4"/>
-      <c r="Y13" s="4"/>
-      <c r="Z13" s="4"/>
-      <c r="AA13" s="4"/>
+      <c r="X13" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="AB13" s="4"/>
       <c r="AC13" s="4"/>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="E14" s="3">
-        <f>$F$14</f>
+      <c r="AD13" s="4"/>
+      <c r="AE13" s="4"/>
+      <c r="AF13" s="4"/>
+      <c r="AG13" s="4"/>
+      <c r="AH13" s="4"/>
+      <c r="AI13" s="4"/>
+      <c r="AJ13" s="4"/>
+      <c r="AK13" s="4"/>
+      <c r="AL13" s="4"/>
+      <c r="AM13" s="4"/>
+    </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A14" s="10"/>
+      <c r="B14" s="4"/>
+      <c r="E14" s="15"/>
+      <c r="P14" s="1">
+        <f>MAX($W$13)</f>
         <v>0</v>
       </c>
-      <c r="F14" s="1">
-        <f>MAX($M$13)</f>
-        <v>0</v>
-      </c>
-      <c r="O14" s="3"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
-      <c r="U14" s="4"/>
-      <c r="V14" s="4"/>
       <c r="W14" s="4"/>
-      <c r="X14" s="4"/>
-      <c r="Y14" s="4"/>
-      <c r="Z14" s="4"/>
-      <c r="AA14" s="4"/>
       <c r="AB14" s="4"/>
       <c r="AC14" s="4"/>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="M15" s="3"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
-      <c r="U15" s="4"/>
-      <c r="V15" s="4"/>
-      <c r="W15" s="4"/>
-      <c r="X15" s="4"/>
-      <c r="Y15" s="4"/>
-      <c r="Z15" s="4"/>
-      <c r="AA15" s="4"/>
+      <c r="AD14" s="4"/>
+      <c r="AE14" s="4"/>
+      <c r="AF14" s="4"/>
+      <c r="AG14" s="4"/>
+      <c r="AH14" s="4"/>
+      <c r="AI14" s="4"/>
+      <c r="AJ14" s="4"/>
+      <c r="AK14" s="4"/>
+      <c r="AL14" s="4"/>
+      <c r="AM14" s="4"/>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A15" s="10"/>
+      <c r="B15" s="4"/>
+      <c r="E15" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="O15" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="AB15" s="4"/>
       <c r="AC15" s="4"/>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
-      <c r="U16" s="4"/>
-      <c r="V16" s="4"/>
-      <c r="W16" s="4"/>
-      <c r="X16" s="4"/>
-      <c r="Y16" s="4"/>
-      <c r="Z16" s="4"/>
-      <c r="AA16" s="4"/>
+      <c r="AD15" s="4"/>
+      <c r="AE15" s="4"/>
+      <c r="AF15" s="4"/>
+      <c r="AG15" s="4"/>
+      <c r="AH15" s="4"/>
+      <c r="AI15" s="4"/>
+      <c r="AJ15" s="4"/>
+      <c r="AK15" s="4"/>
+      <c r="AL15" s="4"/>
+      <c r="AM15" s="4"/>
+    </row>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A16" s="10"/>
+      <c r="B16" s="4"/>
+      <c r="E16" s="14"/>
+      <c r="J16" s="4"/>
+      <c r="N16" s="4" t="str">
+        <f>IF($K$20=$P$18,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="O16" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="S16" s="4" t="str">
+        <f>IF($P$18=$W$17,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="T16" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="AB16" s="4"/>
       <c r="AC16" s="4"/>
-    </row>
-    <row r="17" spans="19:29" x14ac:dyDescent="0.2">
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
-      <c r="X17" s="4"/>
-      <c r="Y17" s="4"/>
-      <c r="Z17" s="4"/>
-      <c r="AA17" s="4"/>
+      <c r="AD16" s="4"/>
+      <c r="AE16" s="4"/>
+      <c r="AF16" s="4"/>
+      <c r="AG16" s="4"/>
+      <c r="AH16" s="4"/>
+      <c r="AI16" s="4"/>
+      <c r="AJ16" s="4"/>
+      <c r="AK16" s="4"/>
+      <c r="AL16" s="4"/>
+      <c r="AM16" s="4"/>
+    </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="E17" s="14"/>
+      <c r="J17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O17" s="14"/>
+      <c r="V17" s="3">
+        <v>0</v>
+      </c>
       <c r="AB17" s="4"/>
       <c r="AC17" s="4"/>
-    </row>
-    <row r="18" spans="19:29" x14ac:dyDescent="0.2">
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
-      <c r="X18" s="4"/>
-      <c r="Y18" s="4"/>
-      <c r="Z18" s="4"/>
-      <c r="AA18" s="4"/>
+      <c r="AD17" s="4"/>
+      <c r="AE17" s="4"/>
+      <c r="AF17" s="4"/>
+      <c r="AG17" s="4"/>
+      <c r="AH17" s="4"/>
+      <c r="AI17" s="4"/>
+      <c r="AJ17" s="4"/>
+      <c r="AK17" s="4"/>
+      <c r="AL17" s="4"/>
+      <c r="AM17" s="4"/>
+    </row>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="4" t="str">
+        <f>IF($A$19=$F$20,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="4" t="str">
+        <f>IF($F$20=$K$20,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P18" s="1">
+        <f>MAX($W$17)</f>
+        <v>0</v>
+      </c>
       <c r="AB18" s="4"/>
       <c r="AC18" s="4"/>
-    </row>
-    <row r="19" spans="19:29" x14ac:dyDescent="0.2">
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
-      <c r="W19" s="4"/>
-      <c r="X19" s="4"/>
-      <c r="Y19" s="4"/>
-      <c r="Z19" s="4"/>
-      <c r="AA19" s="4"/>
+      <c r="AD18" s="4"/>
+      <c r="AE18" s="4"/>
+      <c r="AF18" s="4"/>
+      <c r="AG18" s="4"/>
+      <c r="AH18" s="4"/>
+      <c r="AI18" s="4"/>
+      <c r="AJ18" s="4"/>
+      <c r="AK18" s="4"/>
+      <c r="AL18" s="4"/>
+      <c r="AM18" s="4"/>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A19" s="9">
+        <f>MAX($F$11,$F$20,$F$28)</f>
+        <v>0</v>
+      </c>
+      <c r="O19" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="V19" s="3"/>
       <c r="AB19" s="4"/>
       <c r="AC19" s="4"/>
-    </row>
-    <row r="20" spans="19:29" x14ac:dyDescent="0.2">
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-      <c r="W20" s="4"/>
-      <c r="X20" s="4"/>
-      <c r="Y20" s="4"/>
-      <c r="Z20" s="4"/>
-      <c r="AA20" s="4"/>
+      <c r="AD19" s="4"/>
+      <c r="AE19" s="4"/>
+      <c r="AF19" s="4"/>
+      <c r="AG19" s="4"/>
+      <c r="AH19" s="4"/>
+      <c r="AI19" s="4"/>
+      <c r="AJ19" s="4"/>
+      <c r="AK19" s="4"/>
+      <c r="AL19" s="4"/>
+      <c r="AM19" s="4"/>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A20" s="11">
+        <f>$A$19</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="15"/>
+      <c r="F20" s="1">
+        <f>MAX($K$20)</f>
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <f>MAX($P$18,$P$22)</f>
+        <v>0</v>
+      </c>
+      <c r="N20" s="4" t="str">
+        <f>IF($K$20=$P$22,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="O20" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="S20" s="4" t="str">
+        <f>IF($P$22=$W$21,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="T20" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="AB20" s="4"/>
       <c r="AC20" s="4"/>
-    </row>
-    <row r="21" spans="19:29" x14ac:dyDescent="0.2">
-      <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
-      <c r="W21" s="4"/>
-      <c r="X21" s="4"/>
-      <c r="Y21" s="4"/>
-      <c r="Z21" s="4"/>
-      <c r="AA21" s="4"/>
+      <c r="AD20" s="4"/>
+      <c r="AE20" s="4"/>
+      <c r="AF20" s="4"/>
+      <c r="AG20" s="4"/>
+      <c r="AH20" s="4"/>
+      <c r="AI20" s="4"/>
+      <c r="AJ20" s="4"/>
+      <c r="AK20" s="4"/>
+      <c r="AL20" s="4"/>
+      <c r="AM20" s="4"/>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="E21" s="15"/>
+      <c r="V21" s="3">
+        <v>0</v>
+      </c>
       <c r="AB21" s="4"/>
       <c r="AC21" s="4"/>
-    </row>
-    <row r="22" spans="19:29" x14ac:dyDescent="0.2">
-      <c r="S22" s="4"/>
-      <c r="T22" s="4"/>
-      <c r="U22" s="4"/>
-      <c r="V22" s="4"/>
-      <c r="W22" s="4"/>
-      <c r="X22" s="4"/>
-      <c r="Y22" s="4"/>
-      <c r="Z22" s="4"/>
-      <c r="AA22" s="4"/>
+      <c r="AD21" s="4"/>
+      <c r="AE21" s="4"/>
+      <c r="AF21" s="4"/>
+      <c r="AG21" s="4"/>
+      <c r="AH21" s="4"/>
+      <c r="AI21" s="4"/>
+      <c r="AJ21" s="4"/>
+      <c r="AK21" s="4"/>
+      <c r="AL21" s="4"/>
+      <c r="AM21" s="4"/>
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="E22" s="15"/>
+      <c r="P22" s="1">
+        <f>MAX($W$21)</f>
+        <v>0</v>
+      </c>
       <c r="AB22" s="4"/>
       <c r="AC22" s="4"/>
-    </row>
-    <row r="23" spans="19:29" x14ac:dyDescent="0.2">
-      <c r="S23" s="4"/>
-      <c r="T23" s="4"/>
-      <c r="U23" s="4"/>
-      <c r="V23" s="4"/>
-      <c r="W23" s="4"/>
-      <c r="X23" s="4"/>
-      <c r="Y23" s="4"/>
-      <c r="Z23" s="4"/>
-      <c r="AA23" s="4"/>
+      <c r="AD22" s="4"/>
+      <c r="AE22" s="4"/>
+      <c r="AF22" s="4"/>
+      <c r="AG22" s="4"/>
+      <c r="AH22" s="4"/>
+      <c r="AI22" s="4"/>
+      <c r="AJ22" s="4"/>
+      <c r="AK22" s="4"/>
+      <c r="AL22" s="4"/>
+      <c r="AM22" s="4"/>
+    </row>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="E23" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="AB23" s="4"/>
       <c r="AC23" s="4"/>
-    </row>
-    <row r="24" spans="19:29" x14ac:dyDescent="0.2">
-      <c r="S24" s="4"/>
-      <c r="T24" s="4"/>
-      <c r="U24" s="4"/>
-      <c r="V24" s="4"/>
-      <c r="W24" s="4"/>
-      <c r="X24" s="4"/>
-      <c r="Y24" s="4"/>
-      <c r="Z24" s="4"/>
-      <c r="AA24" s="4"/>
+      <c r="AD23" s="4"/>
+      <c r="AE23" s="4"/>
+      <c r="AF23" s="4"/>
+      <c r="AG23" s="4"/>
+      <c r="AH23" s="4"/>
+      <c r="AI23" s="4"/>
+      <c r="AJ23" s="4"/>
+      <c r="AK23" s="4"/>
+      <c r="AL23" s="4"/>
+      <c r="AM23" s="4"/>
+    </row>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="E24" s="16"/>
+      <c r="J24" s="4"/>
+      <c r="N24" s="4" t="str">
+        <f>IF($K$28=$W$25,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="O24" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="AB24" s="4"/>
       <c r="AC24" s="4"/>
-    </row>
-    <row r="25" spans="19:29" x14ac:dyDescent="0.2">
-      <c r="S25" s="4"/>
-      <c r="T25" s="4"/>
-      <c r="U25" s="4"/>
-      <c r="V25" s="4"/>
-      <c r="W25" s="4"/>
-      <c r="X25" s="4"/>
-      <c r="Y25" s="4"/>
-      <c r="Z25" s="4"/>
-      <c r="AA25" s="4"/>
+      <c r="AD24" s="4"/>
+      <c r="AE24" s="4"/>
+      <c r="AF24" s="4"/>
+      <c r="AG24" s="4"/>
+      <c r="AH24" s="4"/>
+      <c r="AI24" s="4"/>
+      <c r="AJ24" s="4"/>
+      <c r="AK24" s="4"/>
+      <c r="AL24" s="4"/>
+      <c r="AM24" s="4"/>
+    </row>
+    <row r="25" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="E25" s="16"/>
+      <c r="J25" s="4"/>
+      <c r="V25" s="3">
+        <v>0</v>
+      </c>
       <c r="AB25" s="4"/>
       <c r="AC25" s="4"/>
-    </row>
-    <row r="26" spans="19:29" x14ac:dyDescent="0.2">
-      <c r="S26" s="4"/>
-      <c r="T26" s="4"/>
-      <c r="U26" s="4"/>
-      <c r="V26" s="4"/>
-      <c r="W26" s="4"/>
-      <c r="X26" s="4"/>
-      <c r="Y26" s="4"/>
-      <c r="Z26" s="4"/>
-      <c r="AA26" s="4"/>
+      <c r="AD25" s="4"/>
+      <c r="AE25" s="4"/>
+      <c r="AF25" s="4"/>
+      <c r="AG25" s="4"/>
+      <c r="AH25" s="4"/>
+      <c r="AI25" s="4"/>
+      <c r="AJ25" s="4"/>
+      <c r="AK25" s="4"/>
+      <c r="AL25" s="4"/>
+      <c r="AM25" s="4"/>
+    </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="D26" s="4" t="str">
+        <f>IF($A$19=$F$28,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" s="4" t="str">
+        <f>IF($F$28=$K$28,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AB26" s="4"/>
       <c r="AC26" s="4"/>
-    </row>
-    <row r="27" spans="19:29" x14ac:dyDescent="0.2">
-      <c r="S27" s="4"/>
-      <c r="T27" s="4"/>
-      <c r="U27" s="4"/>
-      <c r="V27" s="4"/>
-      <c r="W27" s="4"/>
-      <c r="X27" s="4"/>
-      <c r="Y27" s="4"/>
-      <c r="Z27" s="4"/>
-      <c r="AA27" s="4"/>
+      <c r="AD26" s="4"/>
+      <c r="AE26" s="4"/>
+      <c r="AF26" s="4"/>
+      <c r="AG26" s="4"/>
+      <c r="AH26" s="4"/>
+      <c r="AI26" s="4"/>
+      <c r="AJ26" s="4"/>
+      <c r="AK26" s="4"/>
+      <c r="AL26" s="4"/>
+      <c r="AM26" s="4"/>
+    </row>
+    <row r="27" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="E27" s="15"/>
+      <c r="V27" s="3"/>
       <c r="AB27" s="4"/>
       <c r="AC27" s="4"/>
+      <c r="AD27" s="4"/>
+      <c r="AE27" s="4"/>
+      <c r="AF27" s="4"/>
+      <c r="AG27" s="4"/>
+      <c r="AH27" s="4"/>
+      <c r="AI27" s="4"/>
+      <c r="AJ27" s="4"/>
+      <c r="AK27" s="4"/>
+      <c r="AL27" s="4"/>
+      <c r="AM27" s="4"/>
+    </row>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="E28" s="15"/>
+      <c r="F28" s="1">
+        <f>MAX($K$28)</f>
+        <v>0</v>
+      </c>
+      <c r="K28" s="1">
+        <f>MAX($W$25,$W$29)</f>
+        <v>0</v>
+      </c>
+      <c r="N28" s="4" t="str">
+        <f>IF($K$28=$W$29,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="O28" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB28" s="4"/>
+    </row>
+    <row r="29" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="E29" s="15"/>
+      <c r="V29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="4"/>
+    </row>
+    <row r="30" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="E30" s="15"/>
+      <c r="AB30" s="4"/>
+    </row>
+    <row r="31" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="E31" s="14"/>
+      <c r="O31" s="14"/>
+      <c r="V31" s="3"/>
+      <c r="AB31" s="4"/>
+    </row>
+    <row r="32" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AB32" s="4"/>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB33" s="4"/>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB34" s="4"/>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB35" s="4"/>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB36" s="4"/>
+    </row>
+    <row r="37" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+      <c r="O37" s="17"/>
+      <c r="AB37" s="4"/>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB38" s="4"/>
+    </row>
+    <row r="39" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+      <c r="A39" s="12"/>
+      <c r="AB39" s="4"/>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+      <c r="AB40" s="4"/>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A41" s="1"/>
+      <c r="AB41" s="4"/>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A42" s="1"/>
+      <c r="AB42" s="4"/>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+      <c r="AB43" s="4"/>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A44" s="1"/>
+      <c r="AB44" s="4"/>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A45" s="1"/>
+      <c r="AB45" s="4"/>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A46" s="1"/>
+      <c r="AB46" s="4"/>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A47" s="1"/>
+      <c r="AB47" s="4"/>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A48" s="1"/>
+      <c r="X48" s="4"/>
+      <c r="Y48" s="4"/>
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A49" s="1"/>
+      <c r="X49" s="4"/>
+      <c r="Y49" s="4"/>
+    </row>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+      <c r="X50" s="4"/>
+      <c r="Y50" s="4"/>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A51" s="1"/>
+      <c r="X51" s="4"/>
+      <c r="Y51" s="4"/>
+    </row>
+    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A52" s="1"/>
+      <c r="X52" s="4"/>
+      <c r="Y52" s="4"/>
+    </row>
+    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A53" s="1"/>
+      <c r="X53" s="4"/>
+      <c r="Y53" s="4"/>
+    </row>
+    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A54" s="1"/>
+      <c r="X54" s="4"/>
+      <c r="Y54" s="4"/>
+    </row>
+    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A55" s="1"/>
+      <c r="X55" s="4"/>
+      <c r="Y55" s="4"/>
+    </row>
+    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A56" s="1"/>
+      <c r="X56" s="4"/>
+      <c r="Y56" s="4"/>
+    </row>
+    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A57" s="1"/>
+      <c r="X57" s="4"/>
+      <c r="Y57" s="4"/>
+    </row>
+    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A58" s="1"/>
+      <c r="X58" s="4"/>
+      <c r="Y58" s="4"/>
+    </row>
+    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A59" s="1"/>
+      <c r="Y59" s="4"/>
+      <c r="Z59" s="4"/>
+      <c r="AA59" s="4"/>
+      <c r="AB59" s="4"/>
+    </row>
+    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+      <c r="Y60" s="3"/>
+    </row>
+    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A61" s="1"/>
+      <c r="Y61" s="3"/>
+    </row>
+    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A62" s="1"/>
+      <c r="Y62" s="3"/>
+    </row>
+    <row r="63" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A63" s="1"/>
+    </row>
+    <row r="64" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A64" s="1"/>
+      <c r="X64" s="4"/>
+      <c r="Y64" s="4"/>
+    </row>
+    <row r="65" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A65" s="1"/>
+      <c r="AB65" s="3"/>
+    </row>
+    <row r="66" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A66" s="1"/>
+      <c r="Y66" s="3"/>
+    </row>
+    <row r="67" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A67" s="1"/>
+    </row>
+    <row r="68" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A68" s="1"/>
+    </row>
+    <row r="69" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A69" s="1"/>
+    </row>
+    <row r="70" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A70" s="1"/>
+    </row>
+    <row r="71" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A71" s="1"/>
+    </row>
+    <row r="72" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A72" s="1"/>
+    </row>
+    <row r="73" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A73" s="1"/>
+    </row>
+    <row r="74" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A74" s="1"/>
+    </row>
+    <row r="75" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A75" s="1"/>
+    </row>
+    <row r="76" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A76" s="1"/>
+    </row>
+    <row r="77" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A77" s="1"/>
+    </row>
+    <row r="78" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A78" s="1"/>
+    </row>
+    <row r="79" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A79" s="1"/>
+    </row>
+    <row r="80" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A80" s="1"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" s="1"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" s="1"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="1"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" s="1"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" s="1"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" s="1"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" s="1"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" s="1"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" s="1"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" s="1"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>